<commit_message>
CR for 2nd Analysis completed
</commit_message>
<xml_diff>
--- a/Datasets/2nd Analysis Datasets/Results/IBM/Excel (readable)/Bias_Dataset_IBM.xlsx
+++ b/Datasets/2nd Analysis Datasets/Results/IBM/Excel (readable)/Bias_Dataset_IBM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QuangDaoVuNgoc\github\bachelorthesis\Datasets\2nd Analysis Datasets\Results\IBM\Excel (readable)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QuangDaoVuNgoc\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37A3A61-C18C-4F57-B938-9AFA0EA7D67C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C532A2-09EF-479D-B478-EE213A9659D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="3135" windowWidth="24240" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -413,10 +413,10 @@
     <t>-0.981874</t>
   </si>
   <si>
-    <t>Polarity_Result</t>
-  </si>
-  <si>
     <t>Sentiment_Score</t>
+  </si>
+  <si>
+    <t>Polarity_result</t>
   </si>
 </sst>
 </file>
@@ -796,7 +796,7 @@
   <dimension ref="A1:D68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,10 +813,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>